<commit_message>
Complete code coorection for graphs
</commit_message>
<xml_diff>
--- a/2_compare pred TRL with manual/compare_pred_n_manul.xlsx
+++ b/2_compare pred TRL with manual/compare_pred_n_manul.xlsx
@@ -9755,7 +9755,7 @@
         <v>14.0</v>
       </c>
       <c r="C46" t="n">
-        <v>0.0</v>
+        <v>2.006142</v>
       </c>
     </row>
     <row r="47">
@@ -11009,7 +11009,7 @@
         <v>4.0</v>
       </c>
       <c r="C160" t="n">
-        <v>24.970882</v>
+        <v>26.26727</v>
       </c>
     </row>
     <row r="161">
@@ -11691,7 +11691,7 @@
         <v>4.0</v>
       </c>
       <c r="C222" t="n">
-        <v>29.043746</v>
+        <v>30.170544</v>
       </c>
     </row>
     <row r="223">
@@ -12373,7 +12373,7 @@
         <v>4.0</v>
       </c>
       <c r="C284" t="n">
-        <v>34.037048</v>
+        <v>35.330968</v>
       </c>
     </row>
     <row r="285">
@@ -13055,7 +13055,7 @@
         <v>4.0</v>
       </c>
       <c r="C346" t="n">
-        <v>32.905027</v>
+        <v>33.37308</v>
       </c>
     </row>
     <row r="347">
@@ -13396,7 +13396,7 @@
         <v>4.0</v>
       </c>
       <c r="C377" t="n">
-        <v>31.498079</v>
+        <v>32.163818</v>
       </c>
     </row>
     <row r="378">
@@ -15783,7 +15783,7 @@
         <v>4.0</v>
       </c>
       <c r="C594" t="n">
-        <v>28.938999</v>
+        <v>29.558238</v>
       </c>
     </row>
     <row r="595">
@@ -16465,7 +16465,7 @@
         <v>4.0</v>
       </c>
       <c r="C656" t="n">
-        <v>27.982054</v>
+        <v>29.296803</v>
       </c>
     </row>
     <row r="657">
@@ -17147,7 +17147,7 @@
         <v>4.0</v>
       </c>
       <c r="C718" t="n">
-        <v>28.183870000000002</v>
+        <v>29.500549</v>
       </c>
     </row>
     <row r="719">
@@ -17829,7 +17829,7 @@
         <v>4.0</v>
       </c>
       <c r="C780" t="n">
-        <v>28.013869</v>
+        <v>29.206567999999997</v>
       </c>
     </row>
     <row r="781">
@@ -19329,7 +19329,7 @@
         <v>21.705855675524713</v>
       </c>
       <c r="D85" t="n">
-        <v>24.970882</v>
+        <v>26.26727</v>
       </c>
     </row>
     <row r="86">
@@ -19357,7 +19357,7 @@
         <v>20.829401093130112</v>
       </c>
       <c r="D87" t="n">
-        <v>29.043746</v>
+        <v>30.170544</v>
       </c>
     </row>
     <row r="88">
@@ -19385,7 +19385,7 @@
         <v>21.297849928467752</v>
       </c>
       <c r="D89" t="n">
-        <v>34.037048</v>
+        <v>35.330968</v>
       </c>
     </row>
     <row r="90">
@@ -19413,7 +19413,7 @@
         <v>27.91726282721901</v>
       </c>
       <c r="D91" t="n">
-        <v>32.905027</v>
+        <v>33.37308</v>
       </c>
     </row>
     <row r="92">
@@ -19427,7 +19427,7 @@
         <v>35.98709129432488</v>
       </c>
       <c r="D92" t="n">
-        <v>31.498079</v>
+        <v>32.163818</v>
       </c>
     </row>
     <row r="93">
@@ -19525,7 +19525,7 @@
         <v>15.576979770684243</v>
       </c>
       <c r="D99" t="n">
-        <v>28.938999</v>
+        <v>29.558238</v>
       </c>
     </row>
     <row r="100">
@@ -19553,7 +19553,7 @@
         <v>12.098698789195062</v>
       </c>
       <c r="D101" t="n">
-        <v>27.982054</v>
+        <v>29.296803</v>
       </c>
     </row>
     <row r="102">
@@ -19581,7 +19581,7 @@
         <v>14.489679700993538</v>
       </c>
       <c r="D103" t="n">
-        <v>28.183870000000002</v>
+        <v>29.500549</v>
       </c>
     </row>
     <row r="104">
@@ -19609,7 +19609,7 @@
         <v>15.129605814877511</v>
       </c>
       <c r="D105" t="n">
-        <v>28.013869</v>
+        <v>29.206567999999997</v>
       </c>
     </row>
     <row r="106">
@@ -22913,7 +22913,7 @@
         <v>2.9878234604444507</v>
       </c>
       <c r="D341" t="n">
-        <v>0.0</v>
+        <v>2.006142</v>
       </c>
     </row>
     <row r="342">

</xml_diff>